<commit_message>
made with template holder test
</commit_message>
<xml_diff>
--- a/with_template_holder_test_result.xlsx
+++ b/with_template_holder_test_result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniil\geekshop2_server\geekshop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danii\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE5F65C-8A9D-4710-AAB7-97963528F6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850AE57D-19CD-452A-B56D-FD43B4736A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -461,17 +461,17 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4">
-        <v>7.09</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
+      <c r="D2" s="3">
+        <v>7.27</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.23</v>
       </c>
       <c r="F2" s="2">
-        <v>43.72</v>
+        <v>42.64</v>
       </c>
       <c r="G2" s="3">
-        <v>9.64</v>
+        <v>9.6</v>
       </c>
       <c r="H2" s="2">
         <v>250</v>
@@ -490,17 +490,17 @@
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2">
-        <v>7.27</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.23</v>
+      <c r="D3" s="4">
+        <v>7.09</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="F3" s="2">
-        <v>42.64</v>
+        <v>43.72</v>
       </c>
       <c r="G3" s="3">
-        <v>9.6</v>
+        <v>9.64</v>
       </c>
       <c r="H3" s="2">
         <v>250</v>

</xml_diff>